<commit_message>
Update the scripts for optimizing learning rate of CNN
</commit_message>
<xml_diff>
--- a/Face_images/F17vsF35_CNN_10EPOCHS.xlsx
+++ b/Face_images/F17vsF35_CNN_10EPOCHS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Group_Learning\Face_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9007BAC8-C5CE-4337-962C-8C470A810080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFB3DCC-D68C-49EC-88F5-66744A51170A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0A965C3F-D2D2-4289-A74C-F33FA826B274}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0A965C3F-D2D2-4289-A74C-F33FA826B274}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN" sheetId="1" r:id="rId1"/>
@@ -210,16 +210,16 @@
                   <c:v>0.27329545</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.29034090000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.31988634999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.35852269999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.42443195000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,16 +723,16 @@
                   <c:v>3.7499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.7500000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.14750000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2669,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DC03C2-0DC3-490B-997E-200CFCA5BDCB}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2691,30 +2691,190 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="2:3">
+      <c r="B3">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5">
+        <v>0.31818200000000002</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6">
+        <v>0.272727</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7">
+        <v>0.18181800000000001</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9">
+        <v>0.26136399999999999</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10">
+        <v>0.26136399999999999</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11">
+        <v>0.34090900000000002</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12">
+        <v>0.25</v>
+      </c>
+      <c r="C12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14">
+        <v>0.30681799999999998</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16">
+        <v>0.272727</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18">
+        <v>0.272727</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="B19">
+        <v>0.38636399999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20">
+        <v>0.272727</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21">
+        <v>0.204545</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="B22">
+        <v>0.25</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" t="e">
+      <c r="B23">
         <f>AVERAGE(B3:B22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C23" t="e">
+        <v>0.26988629999999997</v>
+      </c>
+      <c r="C23">
         <f>AVERAGE(C3:C22)</f>
-        <v>#DIV/0!</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" t="e">
+      <c r="B24">
         <f>STDEV(B3:B22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24" t="e">
+        <v>4.5585329197128162E-2</v>
+      </c>
+      <c r="C24">
         <f>STDEV(C3:C22)</f>
-        <v>#DIV/0!</v>
+        <v>4.5523273400016301E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2769,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C959F7C-C2BB-45FD-ADC6-6300DF2DCE3F}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2808,6 +2968,18 @@
       <c r="C2">
         <v>0.44318200000000002</v>
       </c>
+      <c r="D2">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="E2">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.272727</v>
+      </c>
+      <c r="G2">
+        <v>0.48863600000000001</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3">
@@ -2816,6 +2988,18 @@
       <c r="C3">
         <v>0.23863599999999999</v>
       </c>
+      <c r="D3">
+        <v>0.25</v>
+      </c>
+      <c r="E3">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="F3">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.48863600000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4">
@@ -2824,6 +3008,18 @@
       <c r="C4">
         <v>0.26136399999999999</v>
       </c>
+      <c r="D4">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="F4">
+        <v>0.25</v>
+      </c>
+      <c r="G4">
+        <v>0.26136399999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5">
@@ -2832,6 +3028,18 @@
       <c r="C5">
         <v>0.25</v>
       </c>
+      <c r="D5">
+        <v>0.227273</v>
+      </c>
+      <c r="E5">
+        <v>0.272727</v>
+      </c>
+      <c r="F5">
+        <v>0.48863600000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.26136399999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6">
@@ -2840,6 +3048,18 @@
       <c r="C6">
         <v>0.227273</v>
       </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0.272727</v>
+      </c>
+      <c r="F6">
+        <v>0.272727</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7">
@@ -2848,6 +3068,18 @@
       <c r="C7">
         <v>0.25</v>
       </c>
+      <c r="D7">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.56818199999999996</v>
+      </c>
+      <c r="F7">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="G7">
+        <v>0.52272700000000005</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8">
@@ -2856,6 +3088,18 @@
       <c r="C8">
         <v>0.26136399999999999</v>
       </c>
+      <c r="D8">
+        <v>0.26136399999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.51136400000000004</v>
+      </c>
+      <c r="F8">
+        <v>0.32954499999999998</v>
+      </c>
+      <c r="G8">
+        <v>0.272727</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9">
@@ -2864,6 +3108,18 @@
       <c r="C9">
         <v>0.64772700000000005</v>
       </c>
+      <c r="D9">
+        <v>0.272727</v>
+      </c>
+      <c r="E9">
+        <v>0.25</v>
+      </c>
+      <c r="F9">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10">
@@ -2872,6 +3128,18 @@
       <c r="C10">
         <v>0.227273</v>
       </c>
+      <c r="D10">
+        <v>0.272727</v>
+      </c>
+      <c r="E10">
+        <v>0.46590900000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.52272700000000005</v>
+      </c>
+      <c r="G10">
+        <v>0.29545500000000002</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="B11">
@@ -2880,6 +3148,18 @@
       <c r="C11">
         <v>0.25</v>
       </c>
+      <c r="D11">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="E11">
+        <v>0.272727</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>0.56818199999999996</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12">
@@ -2888,6 +3168,18 @@
       <c r="C12">
         <v>0.23863599999999999</v>
       </c>
+      <c r="D12">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.26136399999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="G12">
+        <v>0.53409099999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13">
@@ -2896,6 +3188,18 @@
       <c r="C13">
         <v>0.25</v>
       </c>
+      <c r="D13">
+        <v>0.272727</v>
+      </c>
+      <c r="E13">
+        <v>0.52272700000000005</v>
+      </c>
+      <c r="F13">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="G13">
+        <v>0.54545500000000002</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14">
@@ -2904,6 +3208,18 @@
       <c r="C14">
         <v>0.23863599999999999</v>
       </c>
+      <c r="D14">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.25</v>
+      </c>
+      <c r="F14">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="G14">
+        <v>0.38636399999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15">
@@ -2912,6 +3228,18 @@
       <c r="C15">
         <v>0.227273</v>
       </c>
+      <c r="D15">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="E15">
+        <v>0.272727</v>
+      </c>
+      <c r="F15">
+        <v>0.48863600000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16">
@@ -2920,6 +3248,18 @@
       <c r="C16">
         <v>0.23863599999999999</v>
       </c>
+      <c r="D16">
+        <v>0.25</v>
+      </c>
+      <c r="E16">
+        <v>0.36363600000000001</v>
+      </c>
+      <c r="F16">
+        <v>0.25</v>
+      </c>
+      <c r="G16">
+        <v>0.53409099999999998</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="B17">
@@ -2928,6 +3268,18 @@
       <c r="C17">
         <v>0.25</v>
       </c>
+      <c r="D17">
+        <v>0.26136399999999999</v>
+      </c>
+      <c r="E17">
+        <v>0.26136399999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.272727</v>
+      </c>
+      <c r="G17">
+        <v>0.38636399999999999</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18">
@@ -2936,6 +3288,18 @@
       <c r="C18">
         <v>0.25</v>
       </c>
+      <c r="D18">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.29545500000000002</v>
+      </c>
+      <c r="F18">
+        <v>0.52272700000000005</v>
+      </c>
+      <c r="G18">
+        <v>0.26136399999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19">
@@ -2944,6 +3308,18 @@
       <c r="C19">
         <v>0.227273</v>
       </c>
+      <c r="D19">
+        <v>0.30681799999999998</v>
+      </c>
+      <c r="E19">
+        <v>0.23863599999999999</v>
+      </c>
+      <c r="F19">
+        <v>0.477273</v>
+      </c>
+      <c r="G19">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20">
@@ -2952,6 +3328,18 @@
       <c r="C20">
         <v>0.25</v>
       </c>
+      <c r="D20">
+        <v>0.28409099999999998</v>
+      </c>
+      <c r="E20">
+        <v>0.227273</v>
+      </c>
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+      <c r="G20">
+        <v>0.63636400000000004</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21">
@@ -2960,6 +3348,18 @@
       <c r="C21">
         <v>0.23863599999999999</v>
       </c>
+      <c r="D21">
+        <v>0.54545500000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.272727</v>
+      </c>
+      <c r="F21">
+        <v>0.272727</v>
+      </c>
+      <c r="G21">
+        <v>0.29545500000000002</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
@@ -2973,21 +3373,21 @@
         <f>AVERAGE(C2:C21)</f>
         <v>0.27329545</v>
       </c>
-      <c r="D22" t="e">
+      <c r="D22">
         <f>AVERAGE(D2:D21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" t="e">
+        <v>0.29034090000000007</v>
+      </c>
+      <c r="E22">
         <f t="shared" ref="E22:G22" si="0">AVERAGE(E2:E21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" t="e">
+        <v>0.31988634999999999</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" t="e">
+        <v>0.35852269999999997</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.42443195000000011</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3002,21 +3402,21 @@
         <f t="shared" ref="C23:G23" si="1">STDEV(C2:C21)</f>
         <v>9.9372383494703481E-2</v>
       </c>
-      <c r="D23" t="e">
+      <c r="D23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" t="e">
+        <v>8.2726572175354771E-2</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F23" t="e">
+        <v>0.10629871318935696</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G23" t="e">
+        <v>0.10827506299775799</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.12746448466573934</v>
       </c>
     </row>
   </sheetData>
@@ -3030,8 +3430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5A3B8B-B2A9-4489-8F36-60427CF0322D}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -3066,6 +3466,18 @@
       <c r="C2">
         <v>0.4</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3">
@@ -3074,6 +3486,18 @@
       <c r="C3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4">
@@ -3082,12 +3506,36 @@
       <c r="C4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.05</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
@@ -3098,6 +3546,18 @@
       <c r="C6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>0.05</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7">
@@ -3106,6 +3566,18 @@
       <c r="C7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8">
@@ -3114,6 +3586,18 @@
       <c r="C8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9">
@@ -3122,12 +3606,36 @@
       <c r="C9">
         <v>0.3</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -3138,12 +3646,36 @@
       <c r="C11">
         <v>0.05</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>0</v>
       </c>
     </row>
@@ -3154,6 +3686,18 @@
       <c r="C13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>0.05</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14">
@@ -3162,12 +3706,36 @@
       <c r="C14">
         <v>0</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>0</v>
       </c>
     </row>
@@ -3178,6 +3746,18 @@
       <c r="C16">
         <v>0</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.3</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="B17">
@@ -3186,6 +3766,18 @@
       <c r="C17">
         <v>0</v>
       </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18">
@@ -3194,6 +3786,18 @@
       <c r="C18">
         <v>0</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19">
@@ -3202,6 +3806,18 @@
       <c r="C19">
         <v>0</v>
       </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20">
@@ -3210,6 +3826,18 @@
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21">
@@ -3218,6 +3846,18 @@
       <c r="C21">
         <v>0</v>
       </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
@@ -3231,21 +3871,21 @@
         <f t="shared" ref="C22:G22" si="0">AVERAGE(C2:C21)</f>
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="D22" t="e">
+      <c r="D22">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" t="e">
+        <v>0.01</v>
+      </c>
+      <c r="E22">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" t="e">
+        <v>2.7500000000000004E-2</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" t="e">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.14750000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>